<commit_message>
Update agenda and Introduction deck, and move docker to day2 folder
Update agenda and Introduction deck, and move docker to day2 folder
</commit_message>
<xml_diff>
--- a/Agenda/SZ&HK 2 Day Bluemix Enablement Class General.xlsx
+++ b/Agenda/SZ&HK 2 Day Bluemix Enablement Class General.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24135" windowHeight="15165" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24135" windowHeight="12750" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tailor Version" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="68">
   <si>
     <t>AGENDA: Cloud OE/Dev Ops (Technical Bootcamp) -3 day Session</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Intro</t>
   </si>
   <si>
-    <t>Cloud Boot Camp Introduction_ 05302014</t>
-  </si>
-  <si>
     <t>Cloud Basics Overview -- IaaS, PaaS, SaaS, CSP PAtterns, CCRA, Impact on IT, Cloud Strategy, Cloud Architecture Considerations, Development/Operations Considerations, Approaches</t>
   </si>
   <si>
@@ -81,9 +78,6 @@
     <t xml:space="preserve">Class exercise: Using BlueMix, build a Cloud application with server side components and a Web Browser frontend. Use the Demo Built on 4/16 Build the application using Java and a NoSQL db like Mongo. </t>
   </si>
   <si>
-    <t>Demo - Bluemix_05302014</t>
-  </si>
-  <si>
     <t>API's What are they, Impact, API Economy, API Consumption, API Deployment and Management, Architecture Consideration</t>
   </si>
   <si>
@@ -96,21 +90,12 @@
     <t xml:space="preserve">Class Exercise: Build a mobile CRUD frontend  app. (Android), Deploy server side Java App to the Mobile simulator </t>
   </si>
   <si>
-    <t>Demo - BlueMix_Mobile_Demo_Guide_05302014</t>
-  </si>
-  <si>
     <t>Day 3</t>
   </si>
   <si>
     <t>Class and Exercise Recap, provide proof of completion</t>
   </si>
   <si>
-    <t xml:space="preserve">Class Exercise: Build Push Notification into the app from BlueMix to Push data on Units Sold. </t>
-  </si>
-  <si>
-    <t>Demo - CaseStudy_Push Notification Service_05302014</t>
-  </si>
-  <si>
     <t>Cloud Pipeline discussion - Class is encourage to present actual customers they are working with presently. We will discuss how to identify cloud opportunities and potential entry points.</t>
   </si>
   <si>
@@ -126,52 +111,13 @@
     <t>All</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Session 6 - Use case driven solution architecture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do a online Bluemix walkthru </t>
-  </si>
-  <si>
-    <t>Online Bluemix Walk Thru. Mangal to display this to class. - We sort out any Bluemix ID issues.</t>
-  </si>
-  <si>
-    <t>https://console.ng.bluemix.net/</t>
-  </si>
-  <si>
-    <t>Bill</t>
-  </si>
-  <si>
-    <t>Bill &amp; Mangal</t>
-  </si>
-  <si>
-    <t>Mangal</t>
-  </si>
-  <si>
-    <t>Team is given an example and asked to expand and or develop a Cloud Solution for the seniero. 2 Senerios --1 - Hospitality addons, 2 Banking in the cloud.</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>Determine teams in the class. Let them know they will be doing exercises together.</t>
-  </si>
-  <si>
     <t>Class Ends Questions and Answers any topic.</t>
   </si>
   <si>
     <t>Send out sign in sheet, Get all on community space.</t>
-  </si>
-  <si>
-    <t>Cloud Boot Camp Sesssion 2 Cloud Foundry-BlueMix_ v1.0 08212014</t>
-  </si>
-  <si>
-    <t>Session 1 - NewEra Cloud Basics v1</t>
-  </si>
-  <si>
-    <t>Cloud Boot Camp  session 5_Cloud enabled DevOps_3Sep14_v4</t>
   </si>
   <si>
     <t>base</t>
@@ -188,24 +134,12 @@
 Room xxxx, xst Floor @ xxx any street, anytown, anycountry</t>
   </si>
   <si>
-    <t>Make sure to introduce the concept of 12 factor, Design Thinking, Lean Start up Agile Development and how these work together to accelerate development</t>
-  </si>
-  <si>
-    <t>Incubation Lab &amp; Development Factory Walkthru</t>
-  </si>
-  <si>
-    <t>Incubation Lab &amp; Factory Approach long draft v1</t>
-  </si>
-  <si>
     <t>Introduction_to_Containers_8JUNE2015</t>
   </si>
   <si>
     <t>Introduction to Containers -- Dockers</t>
   </si>
   <si>
-    <t>Make this session 2 hrs with a interactive session at the end of the 2nd hr. Show part of Incubation Lab Offering. Describe skills needed for this new kind of developer/</t>
-  </si>
-  <si>
     <t>APIM Cloud Ed Module v2 - 2015-05-27</t>
   </si>
   <si>
@@ -217,11 +151,115 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Sep 12 - 13</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Max &amp; Neo</t>
+    <t>00. Cloud Boot Camp Introduction</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>01. GBS Cloud Strategy and Offerings.pptx</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>02. BlueMix Introduction</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>BlueMix Introduction</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Discussion / Exercise – What's your understanding/involvement of Cloud</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Duration</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Overview about CCRA version 4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Team's expectation and understanding. Determine teams in the class. Let them know they will be doing exercises together.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Overview of Bluemix and team can apply id if they did not.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exercise 1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LabExercise1 - Introduction to Bluemix v2.0 04292015</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Max/Neo</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Try the first exercise</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wake up exercise</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Online Bluemix Walk Thru. </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Class Topic Recap and discussion</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>All</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exercise 2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LabExercise2 - Create an Android App v2.0 05012015</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>We sort out any Bluemix ID issues. Let the team copy the VM if they don't have development background.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Open discussion, brain storm regarding how you are going to us cloud to enhance your client(Bank) IT ecosystem.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exercise 4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>01. IBM Bluemix DevOps</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>How to use Bluemix to support DevOps</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LabExercise4 - IBM DevOpse Services - Web v2.1 04252015</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>All</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Max</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -229,12 +267,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="179" formatCode="h:mm;@"/>
+    <numFmt numFmtId="178" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -286,22 +323,8 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -344,7 +367,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -404,19 +427,8 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="111">
+  <cellStyleXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -522,14 +534,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -545,35 +556,30 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="105" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -586,29 +592,26 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="111">
+  <cellStyles count="110">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -661,11 +664,11 @@
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -718,7 +721,6 @@
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="105" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1056,729 +1058,505 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I72"/>
+  <dimension ref="A2:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11" style="1"/>
-    <col min="2" max="3" width="11.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="63.125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="36.625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="31.125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="11" style="1"/>
+    <col min="1" max="1" width="8.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B2" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B3" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="29"/>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="D3" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="16">
+        <f>SUM(A5:A15)</f>
+        <v>0.34375000000000006</v>
+      </c>
+      <c r="B4" s="13">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="14">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="B5" s="14">
+        <f t="shared" ref="B5:B9" si="0">B4+A5</f>
+        <v>0.40625</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A6" s="14">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="B6" s="14">
+        <f t="shared" si="0"/>
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A7" s="14">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="B7" s="14">
+        <f>B5+A7</f>
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="15">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="B8" s="15">
+        <f t="shared" si="0"/>
+        <v>0.45833333333333337</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="12"/>
+    </row>
+    <row r="9" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="14">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="B9" s="14">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
-        <v>0.35416666666666669</v>
-      </c>
-      <c r="B4" s="30">
-        <f>SUM(B5:B16)</f>
-        <v>0.34374999999999994</v>
-      </c>
-      <c r="C4" s="24">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
-        <v>0.35416666666666669</v>
-      </c>
-      <c r="B5" s="25">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="C5" s="25">
-        <f>C4+B5</f>
-        <v>0.41666666666666663</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
-        <v>0.375</v>
-      </c>
-      <c r="B6" s="25">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="C6" s="25">
-        <f>C5+B6</f>
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G6" s="19" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="B7" s="26">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="C7" s="26">
-        <f>C6+B7</f>
-        <v>0.46875</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="19"/>
-    </row>
-    <row r="8" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
-        <v>0.4375</v>
-      </c>
-      <c r="B8" s="25">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="C8" s="25">
-        <f>C7+B8</f>
-        <v>0.51041666666666663</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G8" s="19"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="B9" s="27">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="C9" s="27">
-        <f>C8+B9</f>
-        <v>0.52083333333333326</v>
-      </c>
-      <c r="D9" s="18" t="s">
+      <c r="E9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="15">
+        <v>6.25E-2</v>
+      </c>
+      <c r="B10" s="15">
+        <f>A10+B9</f>
+        <v>0.5625</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="B10" s="26">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="C10" s="26">
-        <f>C9+B10</f>
-        <v>0.56249999999999989</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>12</v>
-      </c>
+      <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
-        <v>0.5625</v>
-      </c>
-      <c r="B11" s="25">
+    </row>
+    <row r="11" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="14">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="B11" s="14">
+        <f t="shared" ref="B11:B12" si="1">B10+A11</f>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="14">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="B12" s="14">
+        <f t="shared" si="1"/>
+        <v>0.60416666666666674</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="14">
+        <v>6.25E-2</v>
+      </c>
+      <c r="B13" s="14">
+        <f>B12+A13</f>
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="15">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="B14" s="15">
+        <f>B13+A14</f>
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="14">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="C11" s="25">
-        <f>C10+B11</f>
-        <v>0.60416666666666652</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" s="25">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="C12" s="25">
-        <f>C11+B12</f>
-        <v>0.64583333333333315</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="9"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
-        <v>0.625</v>
-      </c>
-      <c r="B13" s="26">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="C13" s="26">
-        <f>C12+B13</f>
-        <v>0.65624999999999978</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-    </row>
-    <row r="14" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="B14" s="25">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="C14" s="25">
-        <f>C13+B14</f>
-        <v>0.69791666666666641</v>
-      </c>
-      <c r="D14" s="5" t="s">
+      <c r="B15" s="14">
+        <f>B14+A15</f>
+        <v>0.71875</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="24"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="26"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="16">
+        <f>SUM(A18:A24)</f>
+        <v>0.32291666666666663</v>
+      </c>
+      <c r="B17" s="13">
+        <f>B4</f>
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C17" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14" s="10"/>
-    </row>
-    <row r="15" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
-      <c r="B15" s="25">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="C15" s="25">
-        <f t="shared" ref="C15:C16" si="0">C14+B15</f>
-        <v>0.71874999999999978</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G15" s="10"/>
-    </row>
-    <row r="16" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
-        <v>0.1875</v>
-      </c>
-      <c r="B16" s="25">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="C16" s="25">
-        <f t="shared" si="0"/>
-        <v>0.73958333333333315</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B17" s="30">
-        <f>SUM(B18:B26)</f>
-        <v>0.35416666666666663</v>
-      </c>
-      <c r="C17" s="24">
-        <f>C4</f>
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="I17" s="12"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
-        <v>0.35416666666666669</v>
-      </c>
-      <c r="B18" s="25">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="14">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G18" s="10"/>
-    </row>
-    <row r="19" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
-        <v>0.375</v>
-      </c>
-      <c r="B19" s="25">
+      <c r="B18" s="14">
+        <f>A18+B17</f>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A19" s="14">
+        <v>6.25E-2</v>
+      </c>
+      <c r="B19" s="14">
+        <f t="shared" ref="B19:B24" si="2">A19+B18</f>
+        <v>0.47916666666666663</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="15">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G19" s="10"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="B20" s="26">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6" t="s">
-        <v>9</v>
-      </c>
+      <c r="B20" s="15">
+        <f t="shared" si="2"/>
+        <v>0.5625</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="3">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="B21" s="25">
+    </row>
+    <row r="21" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="14">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="C21" s="5"/>
+      <c r="B21" s="14">
+        <f t="shared" si="2"/>
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>61</v>
+      </c>
       <c r="D21" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G21" s="10"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="3">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="B22" s="26">
+        <v>37</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="14">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-    </row>
-    <row r="23" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A23" s="3">
-        <v>0.5625</v>
-      </c>
-      <c r="B23" s="25">
+      <c r="B22" s="14">
+        <f t="shared" si="2"/>
+        <v>0.64583333333333326</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="15">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="B23" s="15">
+        <f t="shared" si="2"/>
+        <v>0.65624999999999989</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A24" s="14">
         <v>6.25E-2</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G23" s="10"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="3">
-        <v>0.625</v>
-      </c>
-      <c r="B24" s="25">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="C24" s="5"/>
+      <c r="B24" s="14">
+        <f t="shared" si="2"/>
+        <v>0.71874999999999989</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>62</v>
+      </c>
       <c r="D24" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+    </row>
+    <row r="50" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D50" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E50" s="11">
+        <f>(E60*26)</f>
+        <v>184167.1</v>
+      </c>
+    </row>
+    <row r="51" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D51" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G24" s="10"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="3">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="B25" s="26">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-    </row>
-    <row r="26" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A26" s="3">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="B26" s="25">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G26" s="10"/>
-      <c r="H26" s="13"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B27" s="30">
-        <f>SUM(B28:B34)</f>
-        <v>0.35416666666666663</v>
-      </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-    </row>
-    <row r="28" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A28" s="3">
-        <v>0.35416666666666669</v>
-      </c>
-      <c r="B28" s="25">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G28" s="10"/>
-      <c r="H28" s="8" t="s">
+      <c r="E51" s="11">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="52" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D52" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="3">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="B29" s="26">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-    </row>
-    <row r="30" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A30" s="3">
-        <v>0.4375</v>
-      </c>
-      <c r="B30" s="25">
-        <v>6.25E-2</v>
-      </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="B31" s="26">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="3">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="B32" s="25">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G32" s="10"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="3">
-        <v>0.625</v>
-      </c>
-      <c r="B33" s="26">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-    </row>
-    <row r="34" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A34" s="3">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="B34" s="25">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G34" s="10"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="3">
-        <v>0.6875</v>
-      </c>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="15"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B36" s="16"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-    </row>
-    <row r="60" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E60" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F60" s="17">
-        <f>(F70*26)</f>
+      <c r="E52" s="11">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="53" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E53" s="11"/>
+    </row>
+    <row r="54" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E54" s="11"/>
+    </row>
+    <row r="55" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E55" s="11"/>
+    </row>
+    <row r="56" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E56" s="11"/>
+    </row>
+    <row r="57" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E57" s="11">
+        <f>SUM(E50:E56)</f>
+        <v>264167.09999999998</v>
+      </c>
+    </row>
+    <row r="60" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E60" s="1">
+        <v>7083.35</v>
+      </c>
+    </row>
+    <row r="61" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E61" s="1">
+        <f>(E60*2)</f>
+        <v>14166.7</v>
+      </c>
+    </row>
+    <row r="62" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E62" s="1">
+        <f>(E60*26)</f>
         <v>184167.1</v>
       </c>
     </row>
-    <row r="61" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E61" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F61" s="17">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="62" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E62" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F62" s="17">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="63" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="F63" s="17"/>
-    </row>
-    <row r="64" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="F64" s="17"/>
-    </row>
-    <row r="65" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F65" s="17"/>
-    </row>
-    <row r="66" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F66" s="17"/>
-    </row>
-    <row r="67" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F67" s="17">
-        <f>SUM(F60:F66)</f>
-        <v>264167.09999999998</v>
-      </c>
-    </row>
-    <row r="70" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F70" s="1">
-        <v>7083.35</v>
-      </c>
-    </row>
-    <row r="71" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F71" s="1">
-        <f>(F70*2)</f>
-        <v>14166.7</v>
-      </c>
-    </row>
-    <row r="72" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F72" s="1">
-        <f>(F70*26)</f>
-        <v>184167.1</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="G6:G8"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:C3"/>
+  <mergeCells count="2">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A16:F16"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="E16" r:id="rId1" display="www.ace.bluemix.ng"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1805,11 +1583,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="20"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
@@ -1845,7 +1623,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="5"/>
     </row>
@@ -1854,7 +1632,7 @@
         <v>0.5</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" s="6"/>
     </row>
@@ -1863,7 +1641,7 @@
         <v>1.5</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" s="5"/>
     </row>
@@ -1872,7 +1650,7 @@
         <v>0.5</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" s="5"/>
     </row>
@@ -1881,7 +1659,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" s="6"/>
     </row>
@@ -1890,7 +1668,7 @@
         <v>1.5</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" s="5"/>
     </row>
@@ -1899,7 +1677,7 @@
         <v>0.5</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D12" s="6"/>
     </row>
@@ -1908,7 +1686,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D13" s="5"/>
     </row>
@@ -1917,7 +1695,7 @@
         <v>8.5</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D14" s="4"/>
     </row>
@@ -1926,7 +1704,7 @@
         <v>0.5</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" s="5"/>
     </row>
@@ -1935,7 +1713,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16" s="5"/>
     </row>
@@ -1944,7 +1722,7 @@
         <v>0.5</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D17" s="6"/>
     </row>
@@ -1953,7 +1731,7 @@
         <v>1.5</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D18" s="5"/>
     </row>
@@ -1962,7 +1740,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D19" s="6"/>
     </row>
@@ -1971,7 +1749,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D20" s="5"/>
     </row>
@@ -1980,7 +1758,7 @@
         <v>0.5</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D21" s="5"/>
     </row>
@@ -1989,7 +1767,7 @@
         <v>0.5</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22" s="6"/>
     </row>
@@ -1998,7 +1776,7 @@
         <v>1</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D23" s="5"/>
     </row>
@@ -2008,7 +1786,7 @@
         <v>8.5</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D24" s="4"/>
     </row>
@@ -2020,7 +1798,7 @@
         <v>0.5</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D25" s="5"/>
     </row>
@@ -2032,7 +1810,7 @@
         <v>1</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D26" s="5"/>
     </row>
@@ -2044,7 +1822,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D27" s="5"/>
     </row>
@@ -2056,7 +1834,7 @@
         <v>1.5</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D28" s="5"/>
     </row>
@@ -2068,7 +1846,7 @@
         <v>1</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D29" s="6"/>
     </row>
@@ -2080,7 +1858,7 @@
         <v>2</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D30" s="5"/>
     </row>
@@ -2092,7 +1870,7 @@
         <v>0.5</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D31" s="6"/>
     </row>
@@ -2104,7 +1882,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D32" s="5"/>
     </row>
@@ -2114,9 +1892,9 @@
       <c r="D33" s="5"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="16"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
add how to connect to VM
</commit_message>
<xml_diff>
--- a/Agenda/SZ&HK 2 Day Bluemix Enablement Class General.xlsx
+++ b/Agenda/SZ&HK 2 Day Bluemix Enablement Class General.xlsx
@@ -223,14 +223,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Exercise 2</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>LabExercise2 - Create an Android App v2.0 05012015</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>We sort out any Bluemix ID issues. Let the team copy the VM if they don't have development background.</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -260,6 +252,14 @@
   </si>
   <si>
     <t>Max</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exercise</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Using docker</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -269,7 +269,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="h:mm;@"/>
+    <numFmt numFmtId="177" formatCode="h:mm;@"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -577,12 +577,30 @@
     <xf numFmtId="20" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -590,24 +608,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1060,8 +1060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1076,20 +1076,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="18" t="s">
         <v>45</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1113,7 +1113,7 @@
       <c r="B4" s="13">
         <v>0.39583333333333331</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="19" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="4"/>
@@ -1267,7 +1267,7 @@
         <v>52</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
@@ -1326,12 +1326,12 @@
       <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="24"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="26"/>
+      <c r="A16" s="21"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="23"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="16">
@@ -1342,7 +1342,7 @@
         <f>B4</f>
         <v>0.39583333333333331</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="19" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="4"/>
@@ -1366,7 +1366,7 @@
       </c>
       <c r="F18" s="7"/>
     </row>
-    <row r="19" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="14">
         <v>6.25E-2</v>
       </c>
@@ -1375,13 +1375,13 @@
         <v>0.47916666666666663</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F19" s="7"/>
     </row>
@@ -1409,13 +1409,13 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>37</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F21" s="7"/>
     </row>
@@ -1428,13 +1428,13 @@
         <v>0.64583333333333326</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F22" s="7"/>
     </row>
@@ -1462,13 +1462,13 @@
         <v>0.71874999999999989</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F24" s="7"/>
     </row>
@@ -1583,11 +1583,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="20"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="26"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">

</xml_diff>